<commit_message>
"change somthing and add sentence"
</commit_message>
<xml_diff>
--- a/data/sentence.xlsx
+++ b/data/sentence.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,7 +487,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>44809.96066837963</v>
+        <v>44814.77682810185</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -513,7 +513,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44809.96221420139</v>
+        <v>44814.76734414352</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -539,7 +539,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44809.96046599537</v>
+        <v>44814.7760153588</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -565,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44809.96438907408</v>
+        <v>44814.77075734954</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -591,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>44809.96388015046</v>
+        <v>44814.7702228125</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -617,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>44809.95914787037</v>
+        <v>44816.00728251157</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -643,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>44809.96325706018</v>
+        <v>44816.00867809028</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -669,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>44809.96445552084</v>
+        <v>44814.76977856481</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -695,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>44809.96539020833</v>
+        <v>44814.77070542824</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>44809.96356516203</v>
+        <v>44814.7746128125</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -747,7 +747,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>44809.96502439815</v>
+        <v>44816.00769685186</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -773,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>44809.96778563657</v>
+        <v>44814.77207561343</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -800,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>44809.96644730324</v>
+        <v>44814.77248436343</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -826,7 +826,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>44809.96803806529</v>
+        <v>44814.77724549769</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -852,7 +852,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>44809.962886875</v>
+        <v>44814.77501091435</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>44809.96343094907</v>
+        <v>44816.00839300926</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -904,7 +904,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>44809.96036642361</v>
+        <v>44816.00879736111</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -930,7 +930,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>44809.96433440972</v>
+        <v>44814.77160474537</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>44809.96516199074</v>
+        <v>44814.77616778935</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -984,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>44809.96708282407</v>
+        <v>44816.00888778935</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>44809.96716247685</v>
+        <v>44814.77166428241</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1036,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>44809.96747380787</v>
+        <v>44814.77226959491</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1062,7 +1062,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>44809.96655972222</v>
+        <v>44814.77006715278</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>44809.95868418981</v>
+        <v>44816.00448315972</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1115,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>44809.95754172454</v>
+        <v>44814.77435706019</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1141,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>44809.96627965278</v>
+        <v>44814.96243638889</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1167,7 +1167,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>44809.96571232639</v>
+        <v>44814.77139508102</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1193,7 +1193,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>44809.9676340625</v>
+        <v>44814.77274806713</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1219,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>44809.95084273148</v>
+        <v>44814.76999071759</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1245,11 +1245,1046 @@
         <v>1</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>44809.95797041667</v>
+        <v>44814.76836144676</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
           <t>tangel_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>코를 돼지처럼 그려놨어</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>They just can't get my nose right!</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>44814.77115533565</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>tangel_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>너흰 그렇겠지 멋지게 그려 줬으니..</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Well, it's easy for you to say! You guys look amazing.</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>44814.77667180556</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>tangel_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>자, 날 올려줘 위에서 잡아줄께</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>All right, Okay, give me a boost, and I'll pull you up</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>44814.77288965278</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>tangel_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>가방 먼저 줘</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Give us the satchel first.</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>44816.00422657408</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>tangel_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>같이 고생한 게 얼만데 아직도 날 못믿어?</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>I can't believe that after all we've been through together, you don't trust me?</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>44814.96343554398</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>tangel_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>미안! 손에 짐이 많아서..</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Sorry, my hands are full.</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>44811.00312993056</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>tangel_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>가방을 꼭 찾아야 한다!</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Retrieve that satchel at any cost!</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>44814.96381623843</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>tangel_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>넌 내꺼야</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Alone, at last</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>44814.77643712963</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>tangel_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>내가 옷장에 사람을 가둔거야!</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>I've got a person in my closet!</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>44814.77538738426</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>tangel_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>내가 나약하다고요, 엄마?</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Too weak to handel myself out there, huh, mother?</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>44814.77363428241</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>tangel_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>깜짝 선물이 있단다!</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>I have a big surprise</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>44814.7587378125</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>tangel_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>내 선물이 더 놀라울 걸?</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Oh I bet my surprise is bigger.</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>44814.96390042824</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>tangel_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>오 엄마, 저도 드릴 말씀 있어요</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Well mother, there's something I want to tell you.</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>44816.0040205787</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>tangel_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>엄마가 했던말 생각 해 봤는데
+[많이 생각해 봤다 전에 너가 했던말에 대하여]</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Okay, I've been thinking a lot about what you said, earlier.</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>44816.00758071759</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>tangel_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>그 얘긴 관뒀으면 좋겠다</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Because I really thought we dropped the issue, sweetheart</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>44814.76609010417</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>tangel_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>넌 네 앞가림 하긴 너무 약해</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Oh darling, I know you're not strong enough to handle yourself out there</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>44816.00548414352</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>tangel_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>라푼젤, 그 얘긴 그만 하자</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Rapunzel, We're done talking about this</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>44814.76664453703</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>tangel_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>불빛 얘긴 그만 해!
+넌 이 탑을 떠날 수 없어 영원히!</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Enough for the lights, Rapunzel! You are not leaving this tower, ever!</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2" t="n">
+        <v>44816.00618868056</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>tangel_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>'별' 보여달라는 것보단 낫잖아요</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>I just thought it was a better idea than stars</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>44814.75894799769</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>tangel_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>너 혼자 있을 수 있겠니?</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>You sure You'll be all right on your own?</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>44816.00851835648</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>tangel_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>내 주머니 어딨어</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Where is my satchel?</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>44816.01733137731</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>tangel_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>감춰놨지, 절대 못 찾을 곳에</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>I've hidden it, somewhere you'll never find it.</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>44816.02475321759</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>tangel_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>저 항아리에?</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>it's in that pot, isnt it?</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" s="2" t="n">
+        <v>44816.02421196759</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>tangel_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>내 머릴 어쩌려는 거야? 잘라가려고?</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>So, What do you want, with my hair, to cut it?</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2" t="n">
+        <v>44816.02448789352</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>tangel_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>아니야, 내가 원하는건 이 머리카락에서 벗어나는 거야, 진짜로!</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>No! Listen, the only thing I want to do with your hair, is to get out of it. Literally</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>44816.02268734953</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>tangel_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>당신 머리칼을 왜 노려? 
+[왜 지구에서 내가 너의 머리칼을 원해?]</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Why on earth would I want your hair?</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>44816.02372802083</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>tangel_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>그럼 그곳으로 날 안내해 줬다가 집으로 데려다 줘</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Take me to these lanterns, and return me home safely.</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>44816.02175428241</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>tangel_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>이 탑을 다 꺠부수고 박살내도</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>You can tear this tower apart, brick by brick</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" s="2" t="n">
+        <v>44816.0238262037</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>tangel_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>내 도움 없인 그 귀한 주머니 절대 못 찾아</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>But without my help, you will never find your precious satchel.</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>44816.02117099537</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>tangel_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>난 한번 약속하면 절대로 어기지 않아</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>I promise. And when I promise something, I never ever break that promise.</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" s="2" t="n">
+        <v>44816.02362364584</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>tangel_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>소용없어 아무것도 안 보여</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>It's no use. I can't see anything.</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>tangel_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>다 내탓이야. 엄마 말을 진작 들을걸..</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>This is all my fault. She was right</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
+      <c r="E63" s="2" t="n">
+        <v>44816.03170714121</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>tangel_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>내 본명은 유진 피츠허버트야 말해주고 싶었어</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>My real name is Eugene Fitzherbert. Someone might as well know.</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2" t="n">
+        <v>44816.03046299768</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>tangel_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>난 노랠 하면 머리에서 빛이 나</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>I have magic hair that glows when I sing.</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="2" t="n">
+        <v>44816.03134275463</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>tangel_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>살았어 살았다고!</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>I'm alive. I'm alive!</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2" t="n">
+        <v>44816.03107152778</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>tangel_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>안믿었는데.</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>I didn't see that coming.</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>tangel_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>진짜로 막 빛이나
+[진짜 그녀 머리에서 빛이나]</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Her hair actually glows.</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>tangel_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>왜 빛이 나지
+[왜 그녀 머리가 빛나지??]</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Why does her hair glow?</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>tangel_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>빛만 나는게 아니야</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>It doesn't just glow.</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>tangel_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>얘 왜 날 비웃지?</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Why is he smiling at me?</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>44816.03193355976</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>tangel_7</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
"study in office 221010"
</commit_message>
<xml_diff>
--- a/data/sentence.xlsx
+++ b/data/sentence.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,7 +515,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44823.04633702547</v>
+        <v>44844.76965959491</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -542,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44827.76144364583</v>
+        <v>44844.83561008102</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -569,7 +569,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44827.75789586805</v>
+        <v>44844.83495538194</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -704,7 +704,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>44823.04724142361</v>
+        <v>44844.77333452546</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>44824.64506239583</v>
+        <v>44844.77070377315</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -785,7 +785,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>44826.85631509259</v>
+        <v>44844.7803833912</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -894,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>44824.655084375</v>
+        <v>44844.77354201389</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -921,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>44826.83678228009</v>
+        <v>44844.77345179398</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1058,7 +1058,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>44826.8576461574</v>
+        <v>44844.82119972222</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1113,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>44826.84884954861</v>
+        <v>44844.78163292824</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1167,7 +1167,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>44826.83410333333</v>
+        <v>44844.80394146991</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1275,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>44826.85644888889</v>
+        <v>44844.82685549768</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1356,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>44830.77858189647</v>
+        <v>44830.77858189815</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1464,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>44826.83826803241</v>
+        <v>44844.82576273148</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1599,7 +1599,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>44826.8579553125</v>
+        <v>44844.82852371528</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -1626,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>44826.84033783565</v>
+        <v>44844.82908050926</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>44826.8405050463</v>
+        <v>44844.83249679398</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -1763,7 +1763,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>44826.83890255787</v>
+        <v>44844.77856605324</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -1790,7 +1790,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>44826.85597310185</v>
+        <v>44844.77778479167</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -1817,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>44826.83924086805</v>
+        <v>44844.82916106482</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -1898,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>44827.75851872685</v>
+        <v>44844.83259344907</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -1925,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>44823.05104175926</v>
+        <v>44844.76793635417</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -1980,7 +1980,7 @@
         <v>1</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>44827.75841870371</v>
+        <v>44844.82869263889</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -2007,7 +2007,7 @@
         <v>1</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>44826.8561550463</v>
+        <v>44844.79723451389</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -2061,7 +2061,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>44823.04991792824</v>
+        <v>44844.81070938658</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -2088,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="2" t="n">
-        <v>44826.84972877315</v>
+        <v>44844.79402392361</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -2115,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>44826.85737524305</v>
+        <v>44844.79416642361</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -2169,7 +2169,7 @@
         <v>1</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>44826.83933982639</v>
+        <v>44844.77262538194</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -2223,7 +2223,7 @@
         <v>1</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>44826.85816957176</v>
+        <v>44844.80398449074</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -2250,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="E67" s="2" t="n">
-        <v>44824.65315459491</v>
+        <v>44844.77116351852</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -2306,7 +2306,7 @@
         <v>1</v>
       </c>
       <c r="E69" s="2" t="n">
-        <v>44827.75955408565</v>
+        <v>44844.83264717593</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -2360,7 +2360,7 @@
         <v>1</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>44826.85583958333</v>
+        <v>44844.80362780092</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -2387,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>44826.85750798611</v>
+        <v>44844.83548678241</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -2414,7 +2414,7 @@
         <v>1</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>44824.6580821875</v>
+        <v>44844.82676074074</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
@@ -2686,7 +2686,7 @@
         <v>1</v>
       </c>
       <c r="E83" s="2" t="n">
-        <v>44826.85713244213</v>
+        <v>44844.80407037037</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
@@ -2713,7 +2713,7 @@
         <v>1</v>
       </c>
       <c r="E84" s="2" t="n">
-        <v>44826.83969082176</v>
+        <v>44844.77745317129</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -2740,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="E85" s="2" t="n">
-        <v>44826.83870795139</v>
+        <v>44844.79814195602</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
@@ -2767,7 +2767,7 @@
         <v>1</v>
       </c>
       <c r="E86" s="2" t="n">
-        <v>44826.83837199074</v>
+        <v>44844.79907678241</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -2794,7 +2794,7 @@
         <v>1</v>
       </c>
       <c r="E87" s="2" t="n">
-        <v>44826.85790640047</v>
+        <v>44844.83490446759</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
@@ -2821,7 +2821,7 @@
         <v>1</v>
       </c>
       <c r="E88" s="2" t="n">
-        <v>44826.84846340278</v>
+        <v>44844.77707355324</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
@@ -2848,7 +2848,7 @@
         <v>1</v>
       </c>
       <c r="E89" s="2" t="n">
-        <v>44826.8496084375</v>
+        <v>44844.77985939815</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
@@ -2929,7 +2929,7 @@
         <v>1</v>
       </c>
       <c r="E92" s="2" t="n">
-        <v>44826.79264806713</v>
+        <v>44844.77016797454</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -2983,7 +2983,7 @@
         <v>1</v>
       </c>
       <c r="E94" s="2" t="n">
-        <v>44826.79334381944</v>
+        <v>44844.80621981482</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
         <v>1</v>
       </c>
       <c r="E96" s="2" t="n">
-        <v>44826.83305495371</v>
+        <v>44844.77455603009</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -3064,7 +3064,7 @@
         <v>1</v>
       </c>
       <c r="E97" s="2" t="n">
-        <v>44826.79768378472</v>
+        <v>44844.80108430555</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
@@ -3091,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="E98" s="2" t="n">
-        <v>44826.83328048611</v>
+        <v>44844.83616904904</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
@@ -3118,7 +3118,7 @@
         <v>1</v>
       </c>
       <c r="E99" s="2" t="n">
-        <v>44826.80075640047</v>
+        <v>44844.79886037037</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -3145,7 +3145,7 @@
         <v>1</v>
       </c>
       <c r="E100" s="2" t="n">
-        <v>44826.83350818287</v>
+        <v>44844.77286246528</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -3172,7 +3172,7 @@
         <v>1</v>
       </c>
       <c r="E101" s="2" t="n">
-        <v>44826.79739960648</v>
+        <v>44844.82894560185</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
@@ -3199,7 +3199,7 @@
         <v>1</v>
       </c>
       <c r="E102" s="2" t="n">
-        <v>44827.731504375</v>
+        <v>44844.83463002315</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
@@ -3307,7 +3307,7 @@
         <v>1</v>
       </c>
       <c r="E106" s="2" t="n">
-        <v>44827.73593601852</v>
+        <v>44844.83054753472</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
@@ -3361,7 +3361,7 @@
         <v>1</v>
       </c>
       <c r="E108" s="2" t="n">
-        <v>44827.73317847222</v>
+        <v>44844.83522643519</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -3388,7 +3388,7 @@
         <v>1</v>
       </c>
       <c r="E109" s="2" t="n">
-        <v>44827.73502556713</v>
+        <v>44844.83475425926</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
@@ -3415,7 +3415,7 @@
         <v>1</v>
       </c>
       <c r="E110" s="2" t="n">
-        <v>44827.73534579861</v>
+        <v>44844.83307723379</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
@@ -3442,7 +3442,7 @@
         <v>1</v>
       </c>
       <c r="E111" s="2" t="n">
-        <v>44827.75739119213</v>
+        <v>44844.83503821759</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -3717,6 +3717,706 @@
       <c r="F121" t="inlineStr">
         <is>
           <t>tangel_12</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>그렇게 해서 여자애들이 결국 죽는다
+[그게 여자애들이 결국 죽는 방법이야]</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>That's how girls end up dead</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" t="inlineStr"/>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>외국인이랑 우연히 말을 했는데 말을 못 했거든. 그때 배우기로 결심했지
+[요전 날 우연히 외국인과 대화를 나누었는데, 아무 말도 할 수가 없었어요. 그때 나는 영어를 배우기로 결심했다.]</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>The other day, I happened to have a conversation with a foreginer, but I wasmn't able say anything at all. That's when I decided to learn English.</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" t="inlineStr"/>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>학원에 오면 공부를 하지 말고 말을 더 해 독해 말고 그래야 회화가 늘지
+[그냥 읽는 게 아니라 학원이 있는 곳에서 영어를 더 많이 해야 할 것 같아. 그래야 영어 실력이 향상될 거야.]</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>I think you should try to speak english more where you're at the academy, not just read. That's how your english will imporve.</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>0</v>
+      </c>
+      <c r="E124" t="inlineStr"/>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>이번달에는 저축 좀 하나 했는데 뭐 또 다 써버렸지
+[이번 달에 돈을 좀 모을 수 있을 줄 알았는데, 결국 돈을 다 써버렸어.]</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>I thought I could save some money this month, but I ended up spending all my money</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" t="inlineStr"/>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>널 좀 봐, 너 완전 홀딱 젖었어. 그것은 정말 형편없다, 너가 그런사람이다 (누구) 이것을 하기를 원했다
+[널 좀 봐. 흠뻑 젖었군요. 그건 너무 시시해! 네가 하고 싶었던 거야]</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>look at you. You're soaked. That is so lame! You're the on who wanted to do it</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" t="inlineStr"/>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>비 쫄딱 맞았네, 다 젖엇다니까. 뉴스 봤으면 우산 챙겼을 텐데
+[비를 맞았어요. 흠뻑 젖었어요. 내가 그 뉴스를 봤더라면. 난 우산을 가져갔을 거야]</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>I got rained on. I got totally soaked. If I had seen the news. I would've taken an umbrella</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" t="inlineStr"/>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>매일 퇴근하고 운동 갈 거라고 한 사람은 너였던거 같은데
+[퇴근 후에 운동하러 갈 사람은 너였어.]</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>You were the one who was going to go to work out after work</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>0</v>
+      </c>
+      <c r="E128" t="inlineStr"/>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>동생이 게임 중독이 됐는데, 혼낼 수 없어. 내가 게임기를 사줬거든
+[내 남동생은 게임을 좋아했지만, 나는 그것에 대해 그에게 소리지를 수 없다. 그를 위해 그것을 산 사람은 나였다.]</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>My brother has gotten into playing games, but I can't yell at him about it. I was the one who bought it for him</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>0</v>
+      </c>
+      <c r="E129" t="inlineStr"/>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>우리 동네에 있는 소방관들은 아주 섹시한 것으로 소문났다. 내가 그것에 분노하냐고?
+[우리 마을의 소방관들은 덥기로 유명하다. 내가 그걸 원망해?]</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>the firemen in our town have a reputation for being hot. Do I resent that?</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>0</v>
+      </c>
+      <c r="E130" t="inlineStr"/>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>그 사람 평판이 그렇게 좋지는 않더라고 . 너무 믿지는 마 그사람이 하는 말
+[그 사람 평판이 생각보다 좋지 않아요. 그를 너무 믿지 마세요.]</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>You know, his reputation isn't as good as I thought. Don't belive him too much.</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>0</v>
+      </c>
+      <c r="E131" t="inlineStr"/>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>너 오늘따라 왜 친절 한 거야? 너 나한테 잘못한거 있는 거 맞구나
+[왜 나한테 그렇게 잘해 주는 거야? 야, 너 나한테 잘못한 게 틀림없어!]</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Why are you being so nice to me? Hey, you must've done something wrong to me!</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" t="inlineStr"/>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>왜 나만 매일 야근을 해야 하는지 화가 난다니까?
+[매일 밤 늦게까지 일한다는 사실이 원망스러울 수밖에 없다.]</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>I can't help but resent the fact that I've been working late every night.</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>0</v>
+      </c>
+      <c r="E133" t="inlineStr"/>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>그렇게 해야 ~하다
+[그렇게]</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>That's how</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" t="inlineStr"/>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>결국 ~이 되다
+[결국 ~하게 되다]</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>End up</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>0</v>
+      </c>
+      <c r="E135" t="inlineStr"/>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>죽은, 완전, 진짜로
+[죽었어]</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Dead</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>0</v>
+      </c>
+      <c r="E136" t="inlineStr"/>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>보다 Vs 찾다
+[보기 vs 찾기]</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Look at Vs Look for</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>0</v>
+      </c>
+      <c r="E137" t="inlineStr"/>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>습하다, 촉촉하다 젖었다, 홀딱젖엇다
+[습기/습기/습기/습기/습기]</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>humid / Moisture / Wet / Soak</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>0</v>
+      </c>
+      <c r="E138" t="inlineStr"/>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>형편없는, 구리다
+[살집이 좋은]</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>leam</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>0</v>
+      </c>
+      <c r="E139" t="inlineStr"/>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>사람을 강조하는것 너
+[바로 너야]</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>You're the one</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>0</v>
+      </c>
+      <c r="E140" t="inlineStr"/>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>평판, 이미지
+[명성.]</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Reputation</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>0</v>
+      </c>
+      <c r="E141" t="inlineStr"/>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>분노를 하다, 부들부들
+[원망]</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Resent</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>0</v>
+      </c>
+      <c r="E142" t="inlineStr"/>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>저번에
+[요전날]</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>The other day</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>0</v>
+      </c>
+      <c r="E143" t="inlineStr"/>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>비맞았다
+[비를 맞았다.]</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>I got rained on</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>0</v>
+      </c>
+      <c r="E144" t="inlineStr"/>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>화내다
+[야단법석을 떨다]</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>yell it</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>0</v>
+      </c>
+      <c r="E145" t="inlineStr"/>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>나 혼났다 선생님께
+[선생님한테 혼났어요.]</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>I got yelled at by my teacher</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>0</v>
+      </c>
+      <c r="E146" t="inlineStr"/>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>그 상태인것 VS 변한것
+[맞으면 맞으면 맞바꾸다]</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>be Vs get</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>0</v>
+      </c>
+      <c r="E147" t="inlineStr"/>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>존재한다고 믿는다
+[을 믿다]</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>believe in</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>0</v>
+      </c>
+      <c r="E148" t="inlineStr"/>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>잘될거라고 믿는다
+[난 널 믿어]</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>I believe in you</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>0</v>
+      </c>
+      <c r="E149" t="inlineStr"/>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>10월_Nick_Drama Topic 11</t>
         </is>
       </c>
     </row>

</xml_diff>